<commit_message>
Minor paragraph fix, address description add
</commit_message>
<xml_diff>
--- a/Utils/menuExcToHtml.xlsx
+++ b/Utils/menuExcToHtml.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bedoz\Desktop\CodingProjects\VCwebsite\Utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83646479-0C7D-40A3-A739-EB45901A6D6D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0741D1E4-86AD-49AD-8DFB-4EFD1EC110AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27105" windowHeight="12810" xr2:uid="{F80E1D2D-14DA-476C-BCA4-096EF2662374}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="176">
   <si>
     <t>Le Classiche</t>
   </si>
@@ -966,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{597202A8-C792-4049-8C78-72759020BD37}">
   <dimension ref="B1:I114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="J40" sqref="J40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,20 +1009,17 @@
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>156</v>
+        <v>172</v>
       </c>
       <c r="D3" s="8">
-        <v>10.5</v>
+        <v>-1</v>
       </c>
       <c r="G3" t="s">
         <v>35</v>
       </c>
       <c r="H3" t="str">
         <f>B3</f>
-        <v>Grabbs</v>
+        <v>Pizza Baby</v>
       </c>
       <c r="I3" t="s">
         <v>36</v>
@@ -1030,20 +1027,17 @@
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
       <c r="D4" s="8">
-        <v>10.5</v>
+        <v>1.5</v>
       </c>
       <c r="G4" t="s">
         <v>37</v>
       </c>
       <c r="H4" s="1">
         <f>D3</f>
-        <v>10.5</v>
+        <v>-1</v>
       </c>
       <c r="I4" t="s">
         <v>36</v>
@@ -1051,13 +1045,10 @@
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>160</v>
+        <v>174</v>
       </c>
       <c r="D5" s="8">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="F5" t="s">
         <v>39</v>
@@ -1065,83 +1056,56 @@
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="D6" s="8">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F6" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="D7" s="8">
-        <v>10</v>
-      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="8"/>
       <c r="G7" t="s">
         <v>38</v>
       </c>
-      <c r="H7" t="str">
+      <c r="H7">
         <f>C3</f>
-        <v>BASE BIANCA: Gorgonzola - Tomino - Scamorza - Patate - Speck in cottura</v>
+        <v>0</v>
       </c>
       <c r="I7" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B8" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="D8" s="8">
-        <v>10.5</v>
-      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="8"/>
       <c r="F8" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="D9" s="8">
-        <v>8.5</v>
-      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8"/>
       <c r="F9" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>170</v>
-      </c>
-      <c r="D10" s="8">
-        <v>12</v>
-      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="8"/>
       <c r="G10" t="s">
         <v>35</v>
       </c>
       <c r="H10" t="str">
         <f>B4</f>
-        <v>Air Max</v>
+        <v>Pizza Doppio Impasto</v>
       </c>
       <c r="I10" t="s">
         <v>36</v>
@@ -1156,7 +1120,7 @@
       </c>
       <c r="H11" s="1">
         <f>D4</f>
-        <v>10.5</v>
+        <v>1.5</v>
       </c>
       <c r="I11" t="s">
         <v>36</v>
@@ -1179,9 +1143,9 @@
       <c r="G14" t="s">
         <v>38</v>
       </c>
-      <c r="H14" t="str">
+      <c r="H14">
         <f>C4</f>
-        <v>BASE MARGHERITA: Gorgonzola - Patate - Peperoni - Funghi Freschi - Salame Piccante - Origano - Salsa Piccante</v>
+        <v>0</v>
       </c>
       <c r="I14" t="s">
         <v>36</v>
@@ -1203,7 +1167,7 @@
       </c>
       <c r="H17" t="str">
         <f>B5</f>
-        <v>Alice</v>
+        <v>Pizza con farina al Farro Integrale</v>
       </c>
       <c r="I17" t="s">
         <v>36</v>
@@ -1215,7 +1179,7 @@
       </c>
       <c r="H18" s="1">
         <f>D5</f>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="I18" t="s">
         <v>36</v>
@@ -1236,9 +1200,9 @@
       <c r="G21" t="s">
         <v>38</v>
       </c>
-      <c r="H21" t="str">
+      <c r="H21">
         <f>C5</f>
-        <v>BASE ROSSA: Bufala - Pomodorini - Capperi - Origano</v>
+        <v>0</v>
       </c>
       <c r="I21" t="s">
         <v>36</v>
@@ -1268,7 +1232,7 @@
       </c>
       <c r="H24" t="str">
         <f>B6</f>
-        <v>Maronno</v>
+        <v>Pizza con farina Grano Khorasan</v>
       </c>
       <c r="I24" t="s">
         <v>36</v>
@@ -1289,7 +1253,7 @@
       </c>
       <c r="H25" s="2">
         <f>D6</f>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I25" t="s">
         <v>36</v>
@@ -1336,9 +1300,9 @@
       <c r="G28" t="s">
         <v>38</v>
       </c>
-      <c r="H28" t="str">
+      <c r="H28">
         <f>C6</f>
-        <v>BASE MARGHERITA: Friarielli - Scamorza - Salame Piccante</v>
+        <v>0</v>
       </c>
       <c r="I28" t="s">
         <v>36</v>
@@ -1385,9 +1349,9 @@
       <c r="G31" t="s">
         <v>35</v>
       </c>
-      <c r="H31" t="str">
+      <c r="H31">
         <f>B7</f>
-        <v xml:space="preserve">Lo Fanno </v>
+        <v>0</v>
       </c>
       <c r="I31" t="s">
         <v>36</v>
@@ -1408,7 +1372,7 @@
       </c>
       <c r="H32" s="2">
         <f>D7</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="I32" t="s">
         <v>36</v>
@@ -1455,9 +1419,9 @@
       <c r="G35" t="s">
         <v>38</v>
       </c>
-      <c r="H35" t="str">
+      <c r="H35">
         <f>C7</f>
-        <v>BASE MARGHERITA: Peperoni - Funghi Freschi - Salsiccia - Pancetta</v>
+        <v>0</v>
       </c>
       <c r="I35" t="s">
         <v>36</v>
@@ -1504,9 +1468,9 @@
       <c r="G38" t="s">
         <v>35</v>
       </c>
-      <c r="H38" t="str">
+      <c r="H38">
         <f>B8</f>
-        <v>Cribbio</v>
+        <v>0</v>
       </c>
       <c r="I38" t="s">
         <v>36</v>
@@ -1527,7 +1491,7 @@
       </c>
       <c r="H39" s="2">
         <f>D8</f>
-        <v>10.5</v>
+        <v>0</v>
       </c>
       <c r="I39" t="s">
         <v>36</v>
@@ -1574,9 +1538,9 @@
       <c r="G42" t="s">
         <v>38</v>
       </c>
-      <c r="H42" t="str">
+      <c r="H42">
         <f>C8</f>
-        <v>BASE MARGHERITA: Salame Milano - Funghi Chiodini - Scamorza - Brie</v>
+        <v>0</v>
       </c>
       <c r="I42" t="s">
         <v>36</v>
@@ -1619,9 +1583,9 @@
       <c r="G45" t="s">
         <v>35</v>
       </c>
-      <c r="H45" t="str">
+      <c r="H45">
         <f>B9</f>
-        <v>La Boe</v>
+        <v>0</v>
       </c>
       <c r="I45" t="s">
         <v>36</v>
@@ -1636,7 +1600,7 @@
       </c>
       <c r="H46" s="2">
         <f>D9</f>
-        <v>8.5</v>
+        <v>0</v>
       </c>
       <c r="I46" t="s">
         <v>36</v>
@@ -1683,9 +1647,9 @@
       <c r="G49" t="s">
         <v>38</v>
       </c>
-      <c r="H49" t="str">
+      <c r="H49">
         <f>C9</f>
-        <v>BASE ROSSA: Bufala fuori forno - Basilico - Olio di Oliva</v>
+        <v>0</v>
       </c>
       <c r="I49" t="s">
         <v>36</v>
@@ -1732,9 +1696,9 @@
       <c r="G52" t="s">
         <v>35</v>
       </c>
-      <c r="H52" t="str">
+      <c r="H52">
         <f>B10</f>
-        <v>La Crossfit</v>
+        <v>0</v>
       </c>
       <c r="I52" t="s">
         <v>36</v>
@@ -1755,7 +1719,7 @@
       </c>
       <c r="H53" s="2">
         <f>D10</f>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="I53" t="s">
         <v>36</v>
@@ -1802,9 +1766,9 @@
       <c r="G56" t="s">
         <v>38</v>
       </c>
-      <c r="H56" t="str">
+      <c r="H56">
         <f>C10</f>
-        <v>BASE BIANCA con Farina Grano Khorasan: Stracchino - Bresaola - Grana - Pinoli</v>
+        <v>0</v>
       </c>
       <c r="I56" t="s">
         <v>36</v>
@@ -2495,13 +2459,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="B94:D95"/>
     <mergeCell ref="B99:D100"/>
     <mergeCell ref="B109:D110"/>
     <mergeCell ref="B23:D24"/>
     <mergeCell ref="B45:D46"/>
     <mergeCell ref="B1:D1"/>
-    <mergeCell ref="F1:I1"/>
-    <mergeCell ref="B94:D95"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
wip, serve dimensione img standard
</commit_message>
<xml_diff>
--- a/Utils/menuExcToHtml.xlsx
+++ b/Utils/menuExcToHtml.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bedoz\Desktop\CodingProjects\VCwebsite\Utils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0741D1E4-86AD-49AD-8DFB-4EFD1EC110AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8616F11-FC9E-4215-9CDB-63C7A2712791}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="27105" windowHeight="12810" xr2:uid="{F80E1D2D-14DA-476C-BCA4-096EF2662374}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="191">
   <si>
     <t>Le Classiche</t>
   </si>
@@ -553,6 +553,51 @@
   </si>
   <si>
     <t>Pizza con farina Grano Khorasan</t>
+  </si>
+  <si>
+    <t>Pizze del Mese</t>
+  </si>
+  <si>
+    <t>Novembre</t>
+  </si>
+  <si>
+    <t>Dicembre</t>
+  </si>
+  <si>
+    <t>Gennaio</t>
+  </si>
+  <si>
+    <t>Febbraio</t>
+  </si>
+  <si>
+    <t>Marzo</t>
+  </si>
+  <si>
+    <t>Aprile</t>
+  </si>
+  <si>
+    <t>Maggio</t>
+  </si>
+  <si>
+    <t>Giugno</t>
+  </si>
+  <si>
+    <t>Luglio</t>
+  </si>
+  <si>
+    <t>Agosto</t>
+  </si>
+  <si>
+    <t>Settembre</t>
+  </si>
+  <si>
+    <t>Ottobre</t>
+  </si>
+  <si>
+    <t>BASE CREMA DI BROCCOLI: Mozzarella - Scamorza - Lardo in concia</t>
+  </si>
+  <si>
+    <t>BASE MARGHERITA: Cardi di Cervia - Brie - Alici</t>
   </si>
 </sst>
 </file>
@@ -644,11 +689,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -964,10 +1009,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{597202A8-C792-4049-8C78-72759020BD37}">
-  <dimension ref="B1:I114"/>
+  <dimension ref="A1:I149"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="C123" sqref="C123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,17 +1026,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="F1" s="12" t="s">
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="F1" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
@@ -1214,19 +1259,19 @@
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
       <c r="F23" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
+      <c r="D24" s="12"/>
       <c r="G24" t="s">
         <v>35</v>
       </c>
@@ -1575,11 +1620,11 @@
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
       <c r="G45" t="s">
         <v>35</v>
       </c>
@@ -1592,9 +1637,9 @@
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B46" s="11"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
       <c r="G46" t="s">
         <v>37</v>
       </c>
@@ -2269,16 +2314,16 @@
       </c>
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B94" s="11" t="s">
+      <c r="B94" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="C94" s="11"/>
-      <c r="D94" s="11"/>
+      <c r="C94" s="12"/>
+      <c r="D94" s="12"/>
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B95" s="11"/>
-      <c r="C95" s="11"/>
-      <c r="D95" s="11"/>
+      <c r="B95" s="12"/>
+      <c r="C95" s="12"/>
+      <c r="D95" s="12"/>
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B96" s="7" t="s">
@@ -2314,16 +2359,16 @@
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B99" s="11" t="s">
+      <c r="B99" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="C99" s="11"/>
-      <c r="D99" s="11"/>
+      <c r="C99" s="12"/>
+      <c r="D99" s="12"/>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B100" s="11"/>
-      <c r="C100" s="11"/>
-      <c r="D100" s="11"/>
+      <c r="B100" s="12"/>
+      <c r="C100" s="12"/>
+      <c r="D100" s="12"/>
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B101" s="7" t="s">
@@ -2414,16 +2459,16 @@
       </c>
     </row>
     <row r="109" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B109" s="11" t="s">
+      <c r="B109" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="C109" s="11"/>
-      <c r="D109" s="11"/>
+      <c r="C109" s="12"/>
+      <c r="D109" s="12"/>
     </row>
     <row r="110" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B110" s="11"/>
-      <c r="C110" s="11"/>
-      <c r="D110" s="11"/>
+      <c r="B110" s="12"/>
+      <c r="C110" s="12"/>
+      <c r="D110" s="12"/>
     </row>
     <row r="111" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B111" s="7" t="s">
@@ -2441,7 +2486,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B113" s="7" t="s">
         <v>174</v>
       </c>
@@ -2449,7 +2494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B114" s="7" t="s">
         <v>175</v>
       </c>
@@ -2457,8 +2502,272 @@
         <v>1</v>
       </c>
     </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B117" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="C117" s="12"/>
+      <c r="D117" s="12"/>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B118" s="12"/>
+      <c r="C118" s="12"/>
+      <c r="D118" s="12"/>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>18</v>
+      </c>
+      <c r="B119" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>18</v>
+      </c>
+      <c r="B120" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>19</v>
+      </c>
+      <c r="B121" t="s">
+        <v>179</v>
+      </c>
+      <c r="C121" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>19</v>
+      </c>
+      <c r="B122" t="s">
+        <v>180</v>
+      </c>
+      <c r="C122" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>19</v>
+      </c>
+      <c r="B123" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>19</v>
+      </c>
+      <c r="B124" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>19</v>
+      </c>
+      <c r="B125" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126">
+        <v>19</v>
+      </c>
+      <c r="B126" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127">
+        <v>19</v>
+      </c>
+      <c r="B127" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128">
+        <v>19</v>
+      </c>
+      <c r="B128" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129">
+        <v>19</v>
+      </c>
+      <c r="B129" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130">
+        <v>19</v>
+      </c>
+      <c r="B130" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131">
+        <v>19</v>
+      </c>
+      <c r="B131" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132">
+        <v>19</v>
+      </c>
+      <c r="B132" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133">
+        <v>20</v>
+      </c>
+      <c r="B133" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134">
+        <v>20</v>
+      </c>
+      <c r="B134" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135">
+        <v>20</v>
+      </c>
+      <c r="B135" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136">
+        <v>20</v>
+      </c>
+      <c r="B136" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137">
+        <v>20</v>
+      </c>
+      <c r="B137" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138">
+        <v>20</v>
+      </c>
+      <c r="B138" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139">
+        <v>20</v>
+      </c>
+      <c r="B139" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140">
+        <v>20</v>
+      </c>
+      <c r="B140" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141">
+        <v>20</v>
+      </c>
+      <c r="B141" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142">
+        <v>20</v>
+      </c>
+      <c r="B142" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143">
+        <v>20</v>
+      </c>
+      <c r="B143" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144">
+        <v>20</v>
+      </c>
+      <c r="B144" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145">
+        <v>21</v>
+      </c>
+      <c r="B145" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146">
+        <v>21</v>
+      </c>
+      <c r="B146" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147">
+        <v>21</v>
+      </c>
+      <c r="B147" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148">
+        <v>21</v>
+      </c>
+      <c r="B148" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B149" t="s">
+        <v>183</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
+    <mergeCell ref="B117:D118"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="B94:D95"/>
     <mergeCell ref="B99:D100"/>

</xml_diff>